<commit_message>
[#130526619] Training Set Import columns are now easier to understand because the slider question direction is now a column separate from the multiple choice impacts. Fixed a bug that occurred whenever you filled in cells for multiple choice responses that don't exist. Now they are just ignored. Added a lot of instructions for the import.
</commit_message>
<xml_diff>
--- a/public/training_sets/imports/Wrapt Training Set Import Template.xlsx
+++ b/public/training_sets/imports/Wrapt Training Set Import Template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>gift_sku</t>
   </si>
@@ -22,13 +22,37 @@
     <t>question_impact</t>
   </si>
   <si>
-    <t>response_impact_1</t>
+    <t>slider_impact_direction</t>
   </si>
   <si>
-    <t>response_impact_2</t>
+    <t>choice_1_impact</t>
   </si>
   <si>
-    <t>etc.</t>
+    <t>choice_2_impact</t>
+  </si>
+  <si>
+    <t>choice_3_impact</t>
+  </si>
+  <si>
+    <t>choice_4_impact</t>
+  </si>
+  <si>
+    <t>choice_5_impact</t>
+  </si>
+  <si>
+    <t>choice_6_impact</t>
+  </si>
+  <si>
+    <t>choice_7_impact</t>
+  </si>
+  <si>
+    <t>choice_8_impact</t>
+  </si>
+  <si>
+    <t>choice_9_impact</t>
+  </si>
+  <si>
+    <t>choice_10_impact</t>
   </si>
 </sst>
 </file>
@@ -88,7 +112,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="5" width="17.14"/>
+    <col customWidth="1" min="4" max="6" width="17.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -110,6 +134,30 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>